<commit_message>
Modify the cash and carry test cases to execute faster
</commit_message>
<xml_diff>
--- a/testData/Hana_T37.xlsx
+++ b/testData/Hana_T37.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCECE87-962D-4D06-84BF-3DB8AAC9DE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0288B4CC-F899-44E1-8E7D-6535DFAB6814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated split payment test data
</commit_message>
<xml_diff>
--- a/testData/Hana_T37.xlsx
+++ b/testData/Hana_T37.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0288B4CC-F899-44E1-8E7D-6535DFAB6814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B812783-99EC-4751-B9FA-DB02798D36DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>custcredit</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>customername</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>custphonenumber1</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,7 +608,7 @@
         <v>21</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>24</v>
@@ -641,10 +641,10 @@
         <v>42</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
@@ -718,13 +718,13 @@
         <v>41</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>